<commit_message>
Updated files to include Gerber and drill files for production and added an additional decoupling capcitor to smooth input to barometer.
</commit_message>
<xml_diff>
--- a/Project Outputs/ReefingCutter_V5.xlsx
+++ b/Project Outputs/ReefingCutter_V5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\ReefingCutter_V5\Project Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA23CBF9-1864-48BA-A4CD-B4604B29ED90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{979B25D4-B283-45DF-BBD5-7F4887E54CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{863AFBF3-E9A7-42FD-B31B-746A1D04C087}"/>
+    <workbookView xWindow="5760" yWindow="24" windowWidth="17280" windowHeight="8880" xr2:uid="{741BF22A-35CA-485E-9099-C526270357B2}"/>
   </bookViews>
   <sheets>
     <sheet name="ReefingCutter_V5" sheetId="1" r:id="rId1"/>
@@ -77,46 +77,46 @@
     <t>Barometer</t>
   </si>
   <si>
+    <t>General Purpose Ceramic Capacitor, 1210, 10uF, 10%, X7R, 15%, 25V</t>
+  </si>
+  <si>
+    <t>C1, C5, C6</t>
+  </si>
+  <si>
+    <t>General Purpose Ceramic Capacitor, 0805, 100nF, 5%, X7R, 0.15, 50V</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 22uF 10V X7R ±20% SMD 1206 +125°C Embossed T/R</t>
+  </si>
+  <si>
+    <t>C3, C4</t>
+  </si>
+  <si>
     <t>Series 102 - 5.00 mm Horizontal Entry Modular with Pressure Clamp WR-TBL, 2 pin</t>
   </si>
   <si>
-    <t>Battery Connector, E-Match Connector</t>
-  </si>
-  <si>
-    <t>General Purpose Ceramic Capacitor, 1210, 10uF, 10%, X7R, 15%, 25V</t>
-  </si>
-  <si>
-    <t>C1, C5</t>
-  </si>
-  <si>
-    <t>General Purpose Ceramic Capacitor, 0805, 100nF, 5%, X7R, 0.15, 50V</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>Cap Ceramic 22uF 10V X7R ±20% SMD 1206 +125°C Embossed T/R</t>
-  </si>
-  <si>
-    <t>C3, C4</t>
+    <t>E-Match, Power</t>
+  </si>
+  <si>
+    <t>Shielded Power Inductor WE-PD2SR, L=3.9 µH</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>LED RED CLEAR CHIP SMD</t>
+  </si>
+  <si>
+    <t>LED</t>
   </si>
   <si>
     <t>TRANS NPN 60V 1A SOT23-3</t>
   </si>
   <si>
-    <t>E-Match MOSFET</t>
-  </si>
-  <si>
-    <t>Shielded Power Inductor WE-PD2SR, L=3.9 µH</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>LED RED CLEAR CHIP SMD</t>
-  </si>
-  <si>
-    <t>LED?</t>
+    <t>MOSFET</t>
   </si>
   <si>
     <t>RES SMD 47K OHM 1% 1/10W 0603</t>
@@ -134,7 +134,7 @@
     <t>IC REG BUCK 3.3V 2A TSOT26</t>
   </si>
   <si>
-    <t>Voltage Reg.</t>
+    <t>Reg.</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBB1D62-D686-4B7C-B26F-4B23AB29E3AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06728F76-546A-4D34-87D8-FA0F75E568D5}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -588,7 +588,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -604,7 +604,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -620,7 +620,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>

</xml_diff>